<commit_message>
Backend changes and moved images
</commit_message>
<xml_diff>
--- a/Sizes ref.xlsx
+++ b/Sizes ref.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="2480" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,8 +100,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -124,7 +128,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="13" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -133,6 +137,8 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -141,6 +147,8 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -470,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F9"/>
+  <dimension ref="B1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -489,25 +497,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="2:6">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>960</v>
-      </c>
-      <c r="D2">
-        <v>640</v>
-      </c>
-      <c r="E2" s="1">
-        <f>D2/C2</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="F2" s="2">
-        <f>D2/C2</f>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
     <row r="3" spans="2:6">
       <c r="B3" t="s">
         <v>1</v>
@@ -519,11 +508,11 @@
         <v>640</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E9" si="0">D3/C3</f>
+        <f t="shared" ref="E3:E5" si="0">D3/C3</f>
         <v>0.56239015817223204</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F9" si="1">D3/C3</f>
+        <f t="shared" ref="F3:F5" si="1">D3/C3</f>
         <v>0.56239015817223204</v>
       </c>
     </row>
@@ -571,58 +560,77 @@
     </row>
     <row r="7" spans="2:6">
       <c r="B7" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>1024</v>
+        <v>960</v>
       </c>
       <c r="D7">
-        <v>768</v>
+        <v>640</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.75</v>
+        <f>D7/C7</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <f>D7/C7</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="D8">
-        <v>1536</v>
+        <v>768</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
+        <f>D8/C8</f>
         <v>0.75</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="1"/>
+        <f>D8/C8</f>
         <v>0.75</v>
       </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>2048</v>
+      </c>
+      <c r="D9">
+        <v>1536</v>
+      </c>
+      <c r="E9" s="1">
+        <f>D9/C9</f>
+        <v>0.75</v>
+      </c>
+      <c r="F9" s="2">
+        <f>D9/C9</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>2732</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>2048</v>
       </c>
-      <c r="E9" s="1">
-        <f t="shared" si="0"/>
+      <c r="E10" s="1">
+        <f>D10/C10</f>
         <v>0.74963396778916547</v>
       </c>
-      <c r="F9" s="2">
-        <f t="shared" si="1"/>
+      <c r="F10" s="2">
+        <f>D10/C10</f>
         <v>0.74963396778916547</v>
       </c>
     </row>

</xml_diff>